<commit_message>
dev: update test sheet
</commit_message>
<xml_diff>
--- a/test/data/air-condition-test-sheet.xlsx
+++ b/test/data/air-condition-test-sheet.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="20">
   <si>
     <t>tag</t>
   </si>
@@ -59,43 +59,34 @@
     <t>weight</t>
   </si>
   <si>
-    <t>p1</t>
+    <t>switcher</t>
   </si>
   <si>
     <t>00p:001</t>
   </si>
   <si>
-    <t>FLOAT32</t>
-  </si>
-  <si>
-    <t>DCBA</t>
-  </si>
-  <si>
-    <t>p2</t>
-  </si>
-  <si>
-    <t>p3</t>
-  </si>
-  <si>
-    <t>p4</t>
-  </si>
-  <si>
-    <t>p5</t>
-  </si>
-  <si>
-    <t>p6</t>
-  </si>
-  <si>
-    <t>p7</t>
-  </si>
-  <si>
-    <t>p8</t>
-  </si>
-  <si>
-    <t>p9</t>
-  </si>
-  <si>
-    <t>p10</t>
+    <t>BOOL</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>temperature</t>
+  </si>
+  <si>
+    <t>UINT16</t>
+  </si>
+  <si>
+    <t>BA</t>
+  </si>
+  <si>
+    <t>exception</t>
+  </si>
+  <si>
+    <t>wind_mode</t>
+  </si>
+  <si>
+    <t>working_mode</t>
   </si>
 </sst>
 </file>
@@ -269,7 +260,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="35">
+  <fills count="36">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -285,6 +276,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -622,7 +619,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -646,16 +643,16 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
@@ -664,89 +661,89 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -760,6 +757,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1287,19 +1287,19 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:J11"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="5"/>
   <cols>
-    <col min="1" max="1" width="4.75" style="1" customWidth="1"/>
+    <col min="1" max="1" width="13.75" style="1" customWidth="1"/>
     <col min="2" max="2" width="8.375" style="1" customWidth="1"/>
     <col min="3" max="3" width="9.025" style="1" customWidth="1"/>
     <col min="4" max="4" width="11.0166666666667" style="1" customWidth="1"/>
-    <col min="5" max="5" width="10.2833333333333" style="1" customWidth="1"/>
+    <col min="5" max="5" width="10.375" style="1" customWidth="1"/>
     <col min="6" max="7" width="9.25" style="1" customWidth="1"/>
     <col min="8" max="8" width="8.375" style="1" customWidth="1"/>
     <col min="9" max="9" width="7" style="1" customWidth="1"/>
@@ -1346,7 +1346,7 @@
         <v>11</v>
       </c>
       <c r="C2" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D2" s="3">
         <v>100</v>
@@ -1358,9 +1358,9 @@
         <v>1</v>
       </c>
       <c r="G2" s="3">
-        <v>2</v>
-      </c>
-      <c r="H2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H2" s="5" t="s">
         <v>12</v>
       </c>
       <c r="I2" s="3" t="s">
@@ -1390,13 +1390,13 @@
         <v>2</v>
       </c>
       <c r="G3" s="3">
-        <v>2</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>12</v>
+        <v>1</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>15</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="J3" s="3">
         <v>1</v>
@@ -1404,7 +1404,7 @@
     </row>
     <row r="4" s="1" customFormat="1" spans="1:10">
       <c r="A4" s="3" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>11</v>
@@ -1422,13 +1422,13 @@
         <v>3</v>
       </c>
       <c r="G4" s="3">
-        <v>2</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>12</v>
+        <v>1</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>15</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="J4" s="3">
         <v>1</v>
@@ -1436,7 +1436,7 @@
     </row>
     <row r="5" s="1" customFormat="1" spans="1:10">
       <c r="A5" s="3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>11</v>
@@ -1454,13 +1454,13 @@
         <v>4</v>
       </c>
       <c r="G5" s="3">
-        <v>2</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>12</v>
+        <v>1</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>15</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="J5" s="3">
         <v>1</v>
@@ -1468,7 +1468,7 @@
     </row>
     <row r="6" s="1" customFormat="1" spans="1:10">
       <c r="A6" s="3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>11</v>
@@ -1486,175 +1486,15 @@
         <v>5</v>
       </c>
       <c r="G6" s="3">
-        <v>2</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>12</v>
+        <v>1</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>15</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="J6" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" s="1" customFormat="1" spans="1:10">
-      <c r="A7" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" s="3">
-        <v>3</v>
-      </c>
-      <c r="D7" s="3">
-        <v>100</v>
-      </c>
-      <c r="E7" s="3">
-        <v>1</v>
-      </c>
-      <c r="F7" s="3">
-        <v>6</v>
-      </c>
-      <c r="G7" s="3">
-        <v>2</v>
-      </c>
-      <c r="H7" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="I7" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="J7" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" s="1" customFormat="1" spans="1:10">
-      <c r="A8" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" s="3">
-        <v>3</v>
-      </c>
-      <c r="D8" s="3">
-        <v>100</v>
-      </c>
-      <c r="E8" s="3">
-        <v>1</v>
-      </c>
-      <c r="F8" s="3">
-        <v>7</v>
-      </c>
-      <c r="G8" s="3">
-        <v>2</v>
-      </c>
-      <c r="H8" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="I8" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="J8" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" s="1" customFormat="1" spans="1:10">
-      <c r="A9" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" s="3">
-        <v>3</v>
-      </c>
-      <c r="D9" s="3">
-        <v>100</v>
-      </c>
-      <c r="E9" s="3">
-        <v>1</v>
-      </c>
-      <c r="F9" s="3">
-        <v>8</v>
-      </c>
-      <c r="G9" s="3">
-        <v>2</v>
-      </c>
-      <c r="H9" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="I9" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="J9" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10">
-      <c r="A10" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10" s="3">
-        <v>3</v>
-      </c>
-      <c r="D10" s="3">
-        <v>100</v>
-      </c>
-      <c r="E10" s="3">
-        <v>1</v>
-      </c>
-      <c r="F10" s="3">
-        <v>9</v>
-      </c>
-      <c r="G10" s="3">
-        <v>2</v>
-      </c>
-      <c r="H10" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="I10" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="J10" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10">
-      <c r="A11" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C11" s="3">
-        <v>3</v>
-      </c>
-      <c r="D11" s="3">
-        <v>100</v>
-      </c>
-      <c r="E11" s="3">
-        <v>1</v>
-      </c>
-      <c r="F11" s="3">
-        <v>10</v>
-      </c>
-      <c r="G11" s="3">
-        <v>2</v>
-      </c>
-      <c r="H11" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="I11" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="J11" s="3">
         <v>1</v>
       </c>
     </row>

</xml_diff>